<commit_message>
ajustage des couleurs fichier excel
</commit_message>
<xml_diff>
--- a/Modèle+analyse+SEO+et+accessibilité+(1)(1).xlsx
+++ b/Modèle+analyse+SEO+et+accessibilité+(1)(1).xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="120">
   <si>
     <t>Categorie</t>
   </si>
@@ -52,7 +52,7 @@
     <t> Arborescence des balises H (multi ligne)</t>
   </si>
   <si>
-    <t> Les balises de titre sont imbriqué ou placé selon des règles strictes h1 en premier puis h2 puis h3 etc...pour aider le lecteur a déterminer ou il se trouve au niveau du contenu la page</t>
+    <t>Les balises de titre sont imbriqué ou placé selon des règles strictes h1 en premier puis h2 puis h3 etc...pour aider le lecteur a déterminer ou il se trouve au niveau du contenu la page</t>
   </si>
   <si>
     <t> La balise de titre qui suit h1 est un h3</t>
@@ -67,7 +67,7 @@
     <t>Langage de la Page html ligne 2 lang =default</t>
   </si>
   <si>
-    <t> L'attribut lang de la balise html doit préciser un code langue en 2 ou 3 lettres qui sera hérité à chaque éléments de la page </t>
+    <t>L'attribut lang de la balise html doit préciser un code langue en 2 ou 3 lettres qui sera hérité à chaque éléments de la page </t>
   </si>
   <si>
     <t> La balise html ne précise aucun code langue</t>
@@ -145,6 +145,9 @@
     <t>https://web.dev/link-name/?utm_source=lighthouse&amp;utm_medium=devtools</t>
   </si>
   <si>
+    <t>         &amp;</t>
+  </si>
+  <si>
     <t>SEO</t>
   </si>
   <si>
@@ -259,13 +262,37 @@
     <t>https://web.dev/font-size/</t>
   </si>
   <si>
+    <t>Chevauchement d'élément interactif sur tout les liens du footer</t>
+  </si>
+  <si>
+    <t>Les éléments interactifs doivent avoir une largeur et hauteur suffisante ( 48x48) et avoir également suffisamment d'espace autour d'eux (8px) pour permettre une bonne navigation en mode portable</t>
+  </si>
+  <si>
+    <t>En mode portable les éléments ont que 16 pixel de hauteur </t>
+  </si>
+  <si>
+    <t>Rajouter une propriété padding pour la hauteur pour la largeur/hauteur et une propriété margin pour le chevauchement</t>
+  </si>
+  <si>
+    <t>https://web.dev/tap-targets/?utm_source=lighthouse&amp;utm_medium=devtools</t>
+  </si>
+  <si>
     <t>SEO On-page</t>
   </si>
   <si>
     <t>Elément textuel de la liste du header ligne 55(html) &lt;a&gt;page2&lt;/a&gt;</t>
   </si>
   <si>
-    <t>Mettre des Mots-clés afin d'amélioré le SEO on page </t>
+    <t>Les éléments textuels doivent correspondre au contenu de la page afin d'amélioré la cohérence de la page</t>
+  </si>
+  <si>
+    <t>La deuxième page du site est indiqué avec la mention « page 2 » ce qui n'est pas cohérent pour le visiteur et également pour le référencement naturel</t>
+  </si>
+  <si>
+    <t>Remplacement le champ texte « page 2 » par « nos coordonnees ou notre adresse »</t>
+  </si>
+  <si>
+    <t>https://support.google.com/webmasters/answer/7451184?hl=fr</t>
   </si>
   <si>
     <t>SEO technique</t>
@@ -362,7 +389,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -405,13 +432,40 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="13"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="1"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -421,16 +475,48 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
-        <bgColor rgb="FF993366"/>
+        <bgColor rgb="FF333399"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB2B2B2"/>
+        <bgColor rgb="FFCC9966"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC9966"/>
+        <bgColor rgb="FFB2B2B2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9933FF"/>
+        <bgColor rgb="FF7030A0"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="dashed"/>
+      <right style="dashed"/>
+      <top style="dashed"/>
+      <bottom style="dashed"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -459,7 +545,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -472,15 +558,39 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -509,7 +619,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFB2B2B2"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF7030A0"/>
@@ -542,13 +652,13 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FFCC9966"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF9933FF"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
     </indexedColors>
@@ -561,10 +671,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z44"/>
+  <dimension ref="A1:Z65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B44" activeCellId="0" sqref="B44"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -657,502 +767,534 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+    <row r="5" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+    <row r="7" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F7" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3"/>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A10" s="7"/>
+    </row>
+    <row r="11" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="0" t="s">
+    </row>
+    <row r="13" s="5" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="B13" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="C13" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="D13" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="E13" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="0" t="s">
+      <c r="F13" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="0" t="s">
+    </row>
+    <row r="14" s="5" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="C14" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="D14" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F17" s="0" t="s">
+      <c r="E14" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="0" t="s">
+      <c r="F14" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="0" t="s">
+    </row>
+    <row r="15" s="5" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>49</v>
       </c>
+      <c r="D15" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" s="5" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" s="5" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" s="5" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="E18" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>49</v>
+        <v>62</v>
+      </c>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" s="5" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>57</v>
+        <v>27</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" s="5" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="F21" s="4"/>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>62</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" s="5" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>65</v>
+        <v>77</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="F24" s="0" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="E23" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="F23" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D27" s="0" t="s">
+    </row>
+    <row r="24" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E27" s="0" t="s">
+      <c r="B24" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="F27" s="0" t="s">
+      <c r="C24" s="4" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="B28" s="0" t="s">
+      <c r="D24" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="E24" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="F24" s="4" t="s">
         <v>90</v>
       </c>
+    </row>
+    <row r="25" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" s="5" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="E28" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" s="5" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="F28" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="F29" s="0" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="F31" s="0" t="s">
-        <v>107</v>
-      </c>
-    </row>
+      <c r="B29" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="0" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="0" t="s">
-        <v>110</v>
-      </c>
-    </row>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" display="https://developer.mozilla.org/fr/docs/Web/HTML/Element/Heading_Elements"/>
     <hyperlink ref="F4" r:id="rId2" display="https://developer.mozilla.org/fr/docs/Web/HTTP/Headers/Content-Language"/>
     <hyperlink ref="F5" r:id="rId3" display="https://developer.mozilla.org/fr/docs/Web/HTML/Element/Img"/>
     <hyperlink ref="F6" r:id="rId4" display="https://developer.mozilla.org/fr/docs/Web/HTML/Element/title"/>
-    <hyperlink ref="F8" r:id="rId5" display="https://developer.mozilla.org/en-US/docs/Web/Accessibility/Understanding_WCAG/Perceivable/Color_contrast"/>
-    <hyperlink ref="F9" r:id="rId6" display="https://developer.mozilla.org/en-US/docs/Web/Accessibility/Understanding_WCAG/Perceivable/Color_contrast"/>
-    <hyperlink ref="F10" r:id="rId7" display="https://web.dev/link-name/?utm_source=lighthouse&amp;utm_medium=devtools"/>
-    <hyperlink ref="F16" r:id="rId8" display="https://developer.mozilla.org/fr/docs/Web/HTML/Element"/>
-    <hyperlink ref="F17" r:id="rId9" display="https://fr.wikipedia.org/wiki/Cloaking"/>
-    <hyperlink ref="F18" r:id="rId10" display="https://fr.wikipedia.org/wiki/Cloaking"/>
-    <hyperlink ref="F19" r:id="rId11" display="https://fr.wikipedia.org/wiki/Cloaking"/>
-    <hyperlink ref="F20" r:id="rId12" display="https://fr.wikipedia.org/wiki/Cloaking"/>
-    <hyperlink ref="F22" r:id="rId13" display="https://developer.mozilla.org/fr/docs/Web/HTML/Element/title"/>
-    <hyperlink ref="F23" r:id="rId14" display="https://support.google.com/webmasters/answer/79812?hl=fr"/>
-    <hyperlink ref="F24" r:id="rId15" display="https://developer.mozilla.org/fr/docs/Apprendre/HTML/Introduction_%C3%A0_HTML/The_head_metadata_in_HTML"/>
-    <hyperlink ref="F25" r:id="rId16" display="https://web.dev/font-size/"/>
-    <hyperlink ref="F27" r:id="rId17" display="https://web.dev/uses-webp-images/?utm_source=lighthouse&amp;utm_medium=unknown"/>
-    <hyperlink ref="F28" r:id="rId18" display="https://web.dev/uses-optimized-images/?utm_source=lighthouse&amp;utm_medium=unknown"/>
-    <hyperlink ref="F29" r:id="rId19" display="https://web.dev/unused-css-rules/?utm_source=lighthouse&amp;utm_medium=unknown"/>
-    <hyperlink ref="F31" r:id="rId20" display="https://www.alsacreations.com/astuce/lire/34-charset-iso-8859-1-iso-8859-15-utf-8-lequel-choisir.html"/>
+    <hyperlink ref="F7" r:id="rId5" display="https://developer.mozilla.org/en-US/docs/Web/Accessibility/Understanding_WCAG/Perceivable/Color_contrast"/>
+    <hyperlink ref="F8" r:id="rId6" display="https://developer.mozilla.org/en-US/docs/Web/Accessibility/Understanding_WCAG/Perceivable/Color_contrast"/>
+    <hyperlink ref="F9" r:id="rId7" display="https://web.dev/link-name/?utm_source=lighthouse&amp;utm_medium=devtools"/>
+    <hyperlink ref="F13" r:id="rId8" display="https://developer.mozilla.org/fr/docs/Web/HTML/Element"/>
+    <hyperlink ref="F14" r:id="rId9" display="https://fr.wikipedia.org/wiki/Cloaking"/>
+    <hyperlink ref="F15" r:id="rId10" display="https://fr.wikipedia.org/wiki/Cloaking"/>
+    <hyperlink ref="F16" r:id="rId11" display="https://fr.wikipedia.org/wiki/Cloaking"/>
+    <hyperlink ref="F17" r:id="rId12" display="https://fr.wikipedia.org/wiki/Cloaking"/>
+    <hyperlink ref="F19" r:id="rId13" display="https://developer.mozilla.org/fr/docs/Web/HTML/Element/title"/>
+    <hyperlink ref="F20" r:id="rId14" display="https://support.google.com/webmasters/answer/79812?hl=fr"/>
+    <hyperlink ref="F21" r:id="rId15" display="https://developer.mozilla.org/fr/docs/Apprendre/HTML/Introduction_%C3%A0_HTML/The_head_metadata_in_HTML"/>
+    <hyperlink ref="F22" r:id="rId16" display="https://web.dev/font-size/"/>
+    <hyperlink ref="F23" r:id="rId17" display="https://web.dev/tap-targets/?utm_source=lighthouse&amp;utm_medium=devtools"/>
+    <hyperlink ref="F24" r:id="rId18" display="https://support.google.com/webmasters/answer/7451184?hl=fr"/>
+    <hyperlink ref="F25" r:id="rId19" display="https://web.dev/uses-webp-images/?utm_source=lighthouse&amp;utm_medium=unknown"/>
+    <hyperlink ref="F26" r:id="rId20" display="https://web.dev/uses-optimized-images/?utm_source=lighthouse&amp;utm_medium=unknown"/>
+    <hyperlink ref="F27" r:id="rId21" display="https://web.dev/unused-css-rules/?utm_source=lighthouse&amp;utm_medium=unknown"/>
+    <hyperlink ref="F29" r:id="rId22" display="https://www.alsacreations.com/astuce/lire/34-charset-iso-8859-1-iso-8859-15-utf-8-lequel-choisir.html"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
modif sur les 8 premieres recommandations grisées du document excel
</commit_message>
<xml_diff>
--- a/Modèle+analyse+SEO+et+accessibilité+(1)(1).xlsx
+++ b/Modèle+analyse+SEO+et+accessibilité+(1)(1).xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="120">
   <si>
-    <t>Categorie</t>
+    <t>Catégorie</t>
   </si>
   <si>
     <t>Problème analysé</t>
@@ -133,7 +133,7 @@
     <t> Le orange est utilisé sur d'autre partie du site , le plus simple serait de mettre une couleur plus sombre pour le gris</t>
   </si>
   <si>
-    <t>Texte de lien identique Ligne  230,235,240,245 &lt;span&gt;&lt;/span&gt; Les Texte de lien doivent être discernables , uniques et sélectionnables pour amélioré l'expérience utilisateur lors de la navigation</t>
+    <t>Texte de lien identique Ligne  235,240,245 &lt;span&gt;&lt;/span&gt; Les Texte de lien doivent être discernables , uniques et sélectionnables pour amélioré l'expérience utilisateur lors de la navigation</t>
   </si>
   <si>
     <t>On a un font awesome qui n'est pas considéré comme une image, ni comme un texte mais il est placé dans une balise span qui est une balise inline. Même si il n'y pas de texte a l'intérieur du html, le DOM considère qu'il il y un nœud texte vide a l'intérieur </t>
@@ -674,7 +674,7 @@
   <dimension ref="A1:Z65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>